<commit_message>
Actualización tabla centros de salud
</commit_message>
<xml_diff>
--- a/DATA/Centros_de_salud.xlsx
+++ b/DATA/Centros_de_salud.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34638\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34638\Desktop\El precio de la discapacidad\El-precio-de-la-discapacidad\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12B7B161-91B1-4DB9-9413-55CCCFAA61E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06E8021-9E25-48AE-8981-34A4F57EA92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6CB39A5-3E03-441F-837C-AB6DF80917BE}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="11952" windowHeight="10452" xr2:uid="{E6CB39A5-3E03-441F-837C-AB6DF80917BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -36,18 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>Total de centros</t>
-  </si>
-  <si>
-    <t>Centros de salud</t>
-  </si>
-  <si>
-    <t>Consultorios locales</t>
-  </si>
-  <si>
-    <t>Tasa por 100.000 habitantes</t>
-  </si>
-  <si>
     <t>Andalucía</t>
   </si>
   <si>
@@ -100,6 +88,18 @@
   </si>
   <si>
     <t>Ceuta y Melilla</t>
+  </si>
+  <si>
+    <t>Total_de_centros</t>
+  </si>
+  <si>
+    <t>Centros_de_salud_por_comunidad</t>
+  </si>
+  <si>
+    <t>Consultorios_locales</t>
+  </si>
+  <si>
+    <t>Tasa_por_100.000_habitantes</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,21 +523,21 @@
     <row r="2" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3">
         <v>1517</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4">
         <v>989</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4">
         <v>213</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4">
         <v>162</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
         <v>262</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4">
         <v>166</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>3916</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>1313</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>1207</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>852</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
         <v>526</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
         <v>465</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
         <v>424</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4">
         <v>265</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4">
         <v>296</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5">
         <v>322</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4">
         <v>194</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4">
         <v>7</v>

</xml_diff>